<commit_message>
Finalizado  captura  açoes  envio ao banco  dados
</commit_message>
<xml_diff>
--- a/EmpresasInfomoney.xlsx
+++ b/EmpresasInfomoney.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c113925\OneDrive - Caixa Economica Federal\GENIC-ONEDRIVE\GDP - PANORAMA SEMANAL\acoes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19f4683fa52e751c/CURSO PY BY/pandas/acoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{6025A777-069D-4552-B597-555A34B5BC84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{FEE83E20-F80C-4998-A5DD-BBB38234992E}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{B972571B-B74E-4351-9F43-463091099B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12592552-3DA5-493D-AAE0-8304CEE3592D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0A8344B3-D836-4043-8EC4-DC39D86F9CE7}"/>
+    <workbookView xWindow="-22764" yWindow="1092" windowWidth="21600" windowHeight="11388" xr2:uid="{0A8344B3-D836-4043-8EC4-DC39D86F9CE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Empresas</t>
-  </si>
-  <si>
-    <t>fundo-imobiliario-cxco11</t>
   </si>
   <si>
     <t>ibovespa</t>
@@ -49,17 +46,11 @@
   <si>
     <t>bb-seguridade-bbse3</t>
   </si>
-  <si>
-    <t>porto-seguro-pssa3</t>
-  </si>
-  <si>
-    <t>sulamerica-sula11</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -96,7 +87,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{9ED85102-DB0E-4195-B25B-0A2601B70701}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -405,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E69F0FD1-347D-4E6B-9C46-24D611E7181B}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,32 +417,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>